<commit_message>
add select imput to params
</commit_message>
<xml_diff>
--- a/Rend.xlsx
+++ b/Rend.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="105" windowWidth="20730" windowHeight="9285" activeTab="1"/>
+    <workbookView xWindow="120" yWindow="105" windowWidth="20730" windowHeight="9285"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="2" r:id="rId1"/>
@@ -15,10 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="15">
-  <si>
-    <t>Bloque</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="17">
   <si>
     <t>T1</t>
   </si>
@@ -60,6 +57,15 @@
   </si>
   <si>
     <t>T5 - Exp. + Aceite</t>
+  </si>
+  <si>
+    <t>Trat</t>
+  </si>
+  <si>
+    <t>rep</t>
+  </si>
+  <si>
+    <t>rend seco</t>
   </si>
 </sst>
 </file>
@@ -406,29 +412,29 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:D1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -442,7 +448,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B3">
         <v>2</v>
@@ -456,7 +462,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B4">
         <v>3</v>
@@ -470,7 +476,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5">
         <v>1</v>
@@ -484,7 +490,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B6">
         <v>2</v>
@@ -498,7 +504,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B7">
         <v>3</v>
@@ -512,7 +518,7 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B8">
         <v>1</v>
@@ -526,7 +532,7 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B9">
         <v>2</v>
@@ -540,7 +546,7 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B10">
         <v>3</v>
@@ -554,7 +560,7 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B11">
         <v>1</v>
@@ -568,7 +574,7 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B12">
         <v>2</v>
@@ -582,7 +588,7 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B13">
         <v>3</v>
@@ -596,7 +602,7 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B14">
         <v>1</v>
@@ -610,7 +616,7 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B15">
         <v>2</v>
@@ -624,7 +630,7 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B16">
         <v>3</v>
@@ -645,7 +651,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
@@ -656,21 +662,21 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>8</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B2">
         <v>10.9</v>
@@ -684,7 +690,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B3">
         <v>11.3</v>
@@ -699,7 +705,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B4">
         <v>10.9</v>
@@ -714,7 +720,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B5">
         <v>11.1</v>
@@ -729,7 +735,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B6">
         <v>11.6</v>

</xml_diff>